<commit_message>
update consumption of electricity for transport
</commit_message>
<xml_diff>
--- a/data/database/Data ThreeME-Mex/DataMEX_Emissions.xlsx
+++ b/data/database/Data ThreeME-Mex/DataMEX_Emissions.xlsx
@@ -107,8 +107,8 @@
   </definedNames>
   <calcPr calcId="162913"/>
   <pivotCaches>
-    <pivotCache cacheId="3" r:id="rId17"/>
-    <pivotCache cacheId="4" r:id="rId18"/>
+    <pivotCache cacheId="6" r:id="rId17"/>
+    <pivotCache cacheId="7" r:id="rId18"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -5655,12 +5655,6 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -5668,6 +5662,12 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -5762,6 +5762,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5958,7 +5959,9 @@
               <c:showPercent val="1"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000003-02E0-4C29-BE91-D9066537D6E4}"/>
                 </c:ext>
@@ -6015,7 +6018,9 @@
               </c:spPr>
             </c:leaderLines>
             <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+              </c:ext>
             </c:extLst>
           </c:dLbls>
           <c:cat>
@@ -6110,6 +6115,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -20669,7 +20675,7 @@
             <v>7.051032023618066E-2</v>
           </cell>
           <cell r="E14">
-            <v>3.7637409277196596</v>
+            <v>0.79007274241162662</v>
           </cell>
           <cell r="F14">
             <v>0</v>
@@ -20683,7 +20689,7 @@
             <v>0</v>
           </cell>
           <cell r="E15">
-            <v>4.2269999999999994</v>
+            <v>4.2711168723033835E-2</v>
           </cell>
           <cell r="F15">
             <v>0</v>
@@ -20697,7 +20703,7 @@
             <v>2.6763625993386064E-2</v>
           </cell>
           <cell r="E16">
-            <v>0.53873423370863549</v>
+            <v>0.11308940802019821</v>
           </cell>
           <cell r="F16">
             <v>0</v>
@@ -20711,7 +20717,7 @@
             <v>0.42433590642746566</v>
           </cell>
           <cell r="E17">
-            <v>6.9278152635497392</v>
+            <v>1.4542653464488293</v>
           </cell>
           <cell r="F17">
             <v>0</v>
@@ -20725,7 +20731,7 @@
             <v>0.5902687489971129</v>
           </cell>
           <cell r="E18">
-            <v>8.8823168096311758</v>
+            <v>1.8645482076275635</v>
           </cell>
           <cell r="F18">
             <v>0</v>
@@ -20739,7 +20745,7 @@
             <v>1.5661855452749989E-2</v>
           </cell>
           <cell r="E19">
-            <v>0.872593853719692</v>
+            <v>0.18317217690048124</v>
           </cell>
           <cell r="F19">
             <v>0</v>
@@ -24228,7 +24234,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TablaDinámica8" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TablaDinámica8" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="K4:O159" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="8">
     <pivotField axis="axisRow" multipleItemSelectionAllowed="1" showAll="0">
@@ -24848,7 +24854,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tableau croisé dynamique3" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valeurs" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tableau croisé dynamique3" cacheId="7" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valeurs" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="B2:N31" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="8">
     <pivotField showAll="0"/>
@@ -25099,7 +25105,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tableau croisé dynamique3" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valeurs" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tableau croisé dynamique3" cacheId="7" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valeurs" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="B2:V61" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="8">
     <pivotField showAll="0"/>
@@ -41678,7 +41684,7 @@
   </sheetPr>
   <dimension ref="A1:AA74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G42" sqref="G42"/>
     </sheetView>
   </sheetViews>
@@ -44604,7 +44610,7 @@
   <dimension ref="B2:G14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
@@ -49654,14 +49660,14 @@
         <v>0</v>
       </c>
       <c r="P16" s="10"/>
-      <c r="Q16" s="373" t="s">
+      <c r="Q16" s="371" t="s">
         <v>46</v>
       </c>
-      <c r="R16" s="373"/>
-      <c r="S16" s="373"/>
-      <c r="T16" s="373"/>
-      <c r="U16" s="373"/>
-      <c r="V16" s="373"/>
+      <c r="R16" s="371"/>
+      <c r="S16" s="371"/>
+      <c r="T16" s="371"/>
+      <c r="U16" s="371"/>
+      <c r="V16" s="371"/>
     </row>
     <row r="17" spans="2:22">
       <c r="B17" s="3" t="s">
@@ -49707,12 +49713,12 @@
         <v>0</v>
       </c>
       <c r="P17" s="10"/>
-      <c r="Q17" s="373"/>
-      <c r="R17" s="373"/>
-      <c r="S17" s="373"/>
-      <c r="T17" s="373"/>
-      <c r="U17" s="373"/>
-      <c r="V17" s="373"/>
+      <c r="Q17" s="371"/>
+      <c r="R17" s="371"/>
+      <c r="S17" s="371"/>
+      <c r="T17" s="371"/>
+      <c r="U17" s="371"/>
+      <c r="V17" s="371"/>
     </row>
     <row r="18" spans="2:22">
       <c r="B18" s="3" t="s">
@@ -49758,14 +49764,14 @@
         <v>0</v>
       </c>
       <c r="P18" s="10"/>
-      <c r="Q18" s="374" t="s">
+      <c r="Q18" s="372" t="s">
         <v>50</v>
       </c>
-      <c r="R18" s="374"/>
-      <c r="S18" s="374"/>
-      <c r="T18" s="374"/>
-      <c r="U18" s="374"/>
-      <c r="V18" s="374"/>
+      <c r="R18" s="372"/>
+      <c r="S18" s="372"/>
+      <c r="T18" s="372"/>
+      <c r="U18" s="372"/>
+      <c r="V18" s="372"/>
     </row>
     <row r="19" spans="2:22" ht="15.95" customHeight="1">
       <c r="B19" s="3" t="s">
@@ -50011,14 +50017,14 @@
         <v>0</v>
       </c>
       <c r="P23" s="10"/>
-      <c r="Q23" s="375" t="s">
+      <c r="Q23" s="373" t="s">
         <v>54</v>
       </c>
-      <c r="R23" s="375"/>
-      <c r="S23" s="375"/>
-      <c r="T23" s="375"/>
-      <c r="U23" s="375"/>
-      <c r="V23" s="375"/>
+      <c r="R23" s="373"/>
+      <c r="S23" s="373"/>
+      <c r="T23" s="373"/>
+      <c r="U23" s="373"/>
+      <c r="V23" s="373"/>
     </row>
     <row r="24" spans="2:22">
       <c r="B24" s="3" t="s">
@@ -50064,14 +50070,14 @@
         <v>0</v>
       </c>
       <c r="P24" s="10"/>
-      <c r="Q24" s="371" t="s">
+      <c r="Q24" s="374" t="s">
         <v>56</v>
       </c>
-      <c r="R24" s="371"/>
-      <c r="S24" s="371"/>
-      <c r="T24" s="371"/>
-      <c r="U24" s="371"/>
-      <c r="V24" s="371"/>
+      <c r="R24" s="374"/>
+      <c r="S24" s="374"/>
+      <c r="T24" s="374"/>
+      <c r="U24" s="374"/>
+      <c r="V24" s="374"/>
     </row>
     <row r="25" spans="2:22">
       <c r="B25" s="3" t="s">
@@ -50373,14 +50379,14 @@
         <v>0</v>
       </c>
       <c r="P30" s="10"/>
-      <c r="Q30" s="371" t="s">
+      <c r="Q30" s="374" t="s">
         <v>62</v>
       </c>
-      <c r="R30" s="371"/>
-      <c r="S30" s="371"/>
-      <c r="T30" s="371"/>
-      <c r="U30" s="371"/>
-      <c r="V30" s="371"/>
+      <c r="R30" s="374"/>
+      <c r="S30" s="374"/>
+      <c r="T30" s="374"/>
+      <c r="U30" s="374"/>
+      <c r="V30" s="374"/>
     </row>
     <row r="31" spans="2:22">
       <c r="B31" s="3" t="s">
@@ -50426,14 +50432,14 @@
         <v>0</v>
       </c>
       <c r="P31" s="10"/>
-      <c r="Q31" s="371" t="s">
+      <c r="Q31" s="374" t="s">
         <v>63</v>
       </c>
-      <c r="R31" s="371"/>
-      <c r="S31" s="371"/>
-      <c r="T31" s="371"/>
-      <c r="U31" s="371"/>
-      <c r="V31" s="371"/>
+      <c r="R31" s="374"/>
+      <c r="S31" s="374"/>
+      <c r="T31" s="374"/>
+      <c r="U31" s="374"/>
+      <c r="V31" s="374"/>
     </row>
     <row r="32" spans="2:22">
       <c r="B32" s="3" t="s">
@@ -50479,12 +50485,12 @@
         <v>0</v>
       </c>
       <c r="P32" s="10"/>
-      <c r="Q32" s="371"/>
-      <c r="R32" s="371"/>
-      <c r="S32" s="371"/>
-      <c r="T32" s="371"/>
-      <c r="U32" s="371"/>
-      <c r="V32" s="371"/>
+      <c r="Q32" s="374"/>
+      <c r="R32" s="374"/>
+      <c r="S32" s="374"/>
+      <c r="T32" s="374"/>
+      <c r="U32" s="374"/>
+      <c r="V32" s="374"/>
     </row>
     <row r="33" spans="2:22">
       <c r="B33" s="3" t="s">
@@ -50530,12 +50536,12 @@
         <v>0</v>
       </c>
       <c r="P33" s="10"/>
-      <c r="Q33" s="372"/>
-      <c r="R33" s="372"/>
-      <c r="S33" s="372"/>
-      <c r="T33" s="372"/>
-      <c r="U33" s="372"/>
-      <c r="V33" s="372"/>
+      <c r="Q33" s="375"/>
+      <c r="R33" s="375"/>
+      <c r="S33" s="375"/>
+      <c r="T33" s="375"/>
+      <c r="U33" s="375"/>
+      <c r="V33" s="375"/>
     </row>
     <row r="34" spans="2:22">
       <c r="B34" s="3" t="s">
@@ -55952,17 +55958,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="Q27:V29"/>
+    <mergeCell ref="Q30:V30"/>
+    <mergeCell ref="Q31:V31"/>
+    <mergeCell ref="Q32:V32"/>
+    <mergeCell ref="Q33:V33"/>
     <mergeCell ref="Q25:V26"/>
     <mergeCell ref="Q16:V17"/>
     <mergeCell ref="Q18:V18"/>
     <mergeCell ref="Q19:V21"/>
     <mergeCell ref="Q23:V23"/>
     <mergeCell ref="Q24:V24"/>
-    <mergeCell ref="Q27:V29"/>
-    <mergeCell ref="Q30:V30"/>
-    <mergeCell ref="Q31:V31"/>
-    <mergeCell ref="Q32:V32"/>
-    <mergeCell ref="Q33:V33"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="G3" r:id="rId2" display="INECC@2014"/>
@@ -58987,8 +58993,8 @@
   </sheetPr>
   <dimension ref="B1:K62"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="K58" sqref="K58"/>
+    <sheetView topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="E47" sqref="E47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
@@ -59432,7 +59438,7 @@
       </c>
       <c r="E14" s="219">
         <f>'[2]For ThreeME'!E14</f>
-        <v>3.7637409277196596</v>
+        <v>0.79007274241162662</v>
       </c>
       <c r="F14" s="219">
         <f>'[2]For ThreeME'!F14</f>
@@ -59440,11 +59446,11 @@
       </c>
       <c r="G14" s="220">
         <f t="shared" si="0"/>
-        <v>131.02039524795583</v>
+        <v>128.04672706264782</v>
       </c>
       <c r="H14" s="220">
         <f t="shared" si="1"/>
-        <v>131.02039524795583</v>
+        <v>128.04672706264782</v>
       </c>
       <c r="I14" s="221"/>
       <c r="J14" s="221"/>
@@ -59467,7 +59473,7 @@
       </c>
       <c r="E15" s="219">
         <f>'[2]For ThreeME'!E15</f>
-        <v>4.2269999999999994</v>
+        <v>4.2711168723033835E-2</v>
       </c>
       <c r="F15" s="219">
         <f>'[2]For ThreeME'!F15</f>
@@ -59475,11 +59481,11 @@
       </c>
       <c r="G15" s="220">
         <f t="shared" si="0"/>
-        <v>30.675539000000001</v>
+        <v>26.491250168723035</v>
       </c>
       <c r="H15" s="220">
         <f t="shared" si="1"/>
-        <v>30.675539000000001</v>
+        <v>26.491250168723035</v>
       </c>
       <c r="I15" s="221"/>
       <c r="J15" s="221"/>
@@ -59502,7 +59508,7 @@
       </c>
       <c r="E16" s="219">
         <f>'[2]For ThreeME'!E16</f>
-        <v>0.53873423370863549</v>
+        <v>0.11308940802019821</v>
       </c>
       <c r="F16" s="219">
         <f>'[2]For ThreeME'!F16</f>
@@ -59510,11 +59516,11 @@
       </c>
       <c r="G16" s="220">
         <f t="shared" si="0"/>
-        <v>29.321114859702018</v>
+        <v>28.895470034013581</v>
       </c>
       <c r="H16" s="220">
         <f t="shared" si="1"/>
-        <v>29.321114859702018</v>
+        <v>28.895470034013581</v>
       </c>
       <c r="I16" s="221"/>
       <c r="J16" s="221"/>
@@ -59537,7 +59543,7 @@
       </c>
       <c r="E17" s="219">
         <f>'[2]For ThreeME'!E17</f>
-        <v>6.9278152635497392</v>
+        <v>1.4542653464488293</v>
       </c>
       <c r="F17" s="219">
         <f>'[2]For ThreeME'!F17</f>
@@ -59545,11 +59551,11 @@
       </c>
       <c r="G17" s="220">
         <f t="shared" si="0"/>
-        <v>957.8096614001746</v>
+        <v>952.33611148307364</v>
       </c>
       <c r="H17" s="220">
         <f t="shared" si="1"/>
-        <v>957.8096614001746</v>
+        <v>952.33611148307364</v>
       </c>
       <c r="I17" s="221"/>
       <c r="J17" s="221"/>
@@ -59572,7 +59578,7 @@
       </c>
       <c r="E18" s="219">
         <f>'[2]For ThreeME'!E18</f>
-        <v>8.8823168096311758</v>
+        <v>1.8645482076275635</v>
       </c>
       <c r="F18" s="219">
         <f>'[2]For ThreeME'!F18</f>
@@ -59580,11 +59586,11 @@
       </c>
       <c r="G18" s="220">
         <f t="shared" si="0"/>
-        <v>121.40652616789603</v>
+        <v>114.38875756589242</v>
       </c>
       <c r="H18" s="220">
         <f t="shared" si="1"/>
-        <v>121.40652616789603</v>
+        <v>114.38875756589242</v>
       </c>
       <c r="I18" s="221"/>
       <c r="J18" s="221"/>
@@ -59607,7 +59613,7 @@
       </c>
       <c r="E19" s="219">
         <f>'[2]For ThreeME'!E19</f>
-        <v>0.872593853719692</v>
+        <v>0.18317217690048124</v>
       </c>
       <c r="F19" s="219">
         <f>'[2]For ThreeME'!F19</f>
@@ -59615,11 +59621,11 @@
       </c>
       <c r="G19" s="220">
         <f t="shared" si="0"/>
-        <v>1.4512070812241635</v>
+        <v>0.7617854044049529</v>
       </c>
       <c r="H19" s="220">
         <f t="shared" si="1"/>
-        <v>1.4512070812241635</v>
+        <v>0.7617854044049529</v>
       </c>
       <c r="I19" s="221"/>
       <c r="J19" s="221"/>
@@ -60200,7 +60206,7 @@
       </c>
       <c r="E36" s="223">
         <f t="shared" si="3"/>
-        <v>728.31020590802029</v>
+        <v>707.54586386982305</v>
       </c>
       <c r="F36" s="223">
         <f t="shared" si="3"/>
@@ -60208,11 +60214,11 @@
       </c>
       <c r="G36" s="223">
         <f t="shared" si="3"/>
-        <v>6094.0851496186078</v>
+        <v>6073.3208075804105</v>
       </c>
       <c r="H36" s="223">
         <f t="shared" si="3"/>
-        <v>6030.3027066186078</v>
+        <v>6009.5383645804104</v>
       </c>
       <c r="I36" s="221"/>
       <c r="J36" s="221"/>
@@ -60315,7 +60321,7 @@
       </c>
       <c r="E42" s="223">
         <f t="shared" si="6"/>
-        <v>923.48520590802036</v>
+        <v>902.72086386982301</v>
       </c>
       <c r="F42" s="223">
         <f t="shared" si="6"/>
@@ -60323,11 +60329,11 @@
       </c>
       <c r="G42" s="223">
         <f>G36+G40</f>
-        <v>7848.184821779143</v>
+        <v>7827.4204797409457</v>
       </c>
       <c r="H42" s="223">
         <f>H36+H40</f>
-        <v>7528.9799817791427</v>
+        <v>7508.2156397409453</v>
       </c>
       <c r="I42" s="221"/>
       <c r="J42" s="221"/>
@@ -60435,7 +60441,7 @@
       </c>
       <c r="E47" s="220">
         <f t="shared" si="11"/>
-        <v>25.212201088328904</v>
+        <v>4.4478590501317319</v>
       </c>
       <c r="F47" s="220">
         <f t="shared" si="11"/>
@@ -60443,11 +60449,11 @@
       </c>
       <c r="G47" s="220">
         <f t="shared" si="9"/>
-        <v>1271.6844437569525</v>
+        <v>1250.9201017187554</v>
       </c>
       <c r="H47" s="220">
         <f t="shared" si="10"/>
-        <v>1271.6844437569525</v>
+        <v>1250.9201017187554</v>
       </c>
       <c r="I47" s="221"/>
       <c r="J47" s="221"/>
@@ -60627,7 +60633,7 @@
       </c>
       <c r="E53" s="223">
         <f t="shared" si="17"/>
-        <v>923.48520590802025</v>
+        <v>902.72086386982312</v>
       </c>
       <c r="F53" s="223">
         <f t="shared" si="17"/>
@@ -60635,11 +60641,11 @@
       </c>
       <c r="G53" s="223">
         <f t="shared" si="17"/>
-        <v>7848.184821779143</v>
+        <v>7827.4204797409457</v>
       </c>
       <c r="H53" s="223">
         <f t="shared" si="17"/>
-        <v>7528.9799817791427</v>
+        <v>7508.2156397409453</v>
       </c>
       <c r="I53" s="221"/>
       <c r="J53" s="221"/>
@@ -60708,7 +60714,7 @@
       </c>
       <c r="E58" s="222">
         <f t="shared" si="18"/>
-        <v>6.9278152635497392</v>
+        <v>1.4542653464488293</v>
       </c>
       <c r="F58" s="222">
         <f t="shared" si="18"/>
@@ -60716,11 +60722,11 @@
       </c>
       <c r="G58" s="222">
         <f t="shared" si="18"/>
-        <v>957.8096614001746</v>
+        <v>952.33611148307364</v>
       </c>
       <c r="H58" s="222">
         <f t="shared" si="18"/>
-        <v>957.8096614001746</v>
+        <v>952.33611148307364</v>
       </c>
       <c r="I58" s="221"/>
       <c r="J58" s="221"/>
@@ -60744,7 +60750,7 @@
       </c>
       <c r="E59" s="222">
         <f t="shared" si="19"/>
-        <v>8.8823168096311758</v>
+        <v>1.8645482076275635</v>
       </c>
       <c r="F59" s="222">
         <f t="shared" si="19"/>
@@ -60752,11 +60758,11 @@
       </c>
       <c r="G59" s="222">
         <f t="shared" si="19"/>
-        <v>121.40652616789603</v>
+        <v>114.38875756589242</v>
       </c>
       <c r="H59" s="222">
         <f t="shared" si="19"/>
-        <v>121.40652616789603</v>
+        <v>114.38875756589242</v>
       </c>
       <c r="I59" s="221"/>
       <c r="J59" s="221"/>
@@ -60792,7 +60798,7 @@
       </c>
       <c r="E61" s="228">
         <f t="shared" si="20"/>
-        <v>15.810132073180915</v>
+        <v>3.3188135540763928</v>
       </c>
       <c r="F61" s="228">
         <f t="shared" si="20"/>
@@ -60800,11 +60806,11 @@
       </c>
       <c r="G61" s="228">
         <f t="shared" si="20"/>
-        <v>1079.2161875680706</v>
+        <v>1066.724869048966</v>
       </c>
       <c r="H61" s="228">
         <f t="shared" si="20"/>
-        <v>1079.2161875680706</v>
+        <v>1066.724869048966</v>
       </c>
       <c r="I61" s="221"/>
       <c r="J61" s="221"/>

</xml_diff>